<commit_message>
Them van de khi vao lenh
</commit_message>
<xml_diff>
--- a/ChienLuocGIaoDich/XAUUSD/Bollinger band.xlsx
+++ b/ChienLuocGIaoDich/XAUUSD/Bollinger band.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Xây dựng chiến lược giao dịch cho XAUUSD theo Bollinger band</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Lúc này ngưỡng hỗ trợ đã hình thành, lực mua bắt đầu tăng dần</t>
+  </si>
+  <si>
+    <t>Nếu soi trên khung H4 chắc chắn phải có ít nhất một cây nến vàng được sinh ra, nếu không có hãy cẩn thận</t>
   </si>
 </sst>
 </file>
@@ -160,13 +163,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>18824</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>6024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>12763</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>6024</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,35 +583,40 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="O21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
         <v>14</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="O22" t="s">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>